<commit_message>
refactor: :fire: split project in two
emr files are now in a different project
</commit_message>
<xml_diff>
--- a/cypher/poc.xlsx
+++ b/cypher/poc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renatospaka\dev\heykid\draft\poc\cypher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CCDD07-3290-455E-A5DC-3A963D314E8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC2F260-9286-4969-8B35-F03173C2D37F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="disease" sheetId="3" r:id="rId1"/>
@@ -3466,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A61B1D1-1498-4062-8FF1-43F1DDC4F5BE}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3882,104 +3882,104 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F37" si="2">"MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '" &amp; A2 &amp; "' AND d.vaccine = '" &amp; A2 &amp; "' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);"</f>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG ID' AND d.vaccine = 'BCG ID' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <f>"MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = '" &amp; A2 &amp; "' AND dose.vaccineName = '" &amp; A2 &amp; "' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);"</f>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'BCG ID' AND dose.vaccineName = 'BCG ID' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite B' AND d.vaccine = 'Hepatite B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <f t="shared" ref="F22:F37" si="2">"MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = '" &amp; A3 &amp; "' AND dose.vaccineName = '" &amp; A3 &amp; "' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);"</f>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Hepatite B' AND dose.vaccineName = 'Hepatite B' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPw' AND d.vaccine = 'DTPw' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'DTPw' AND dose.vaccineName = 'DTPw' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F24" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'H Influenzae' AND d.vaccine = 'H Influenzae' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'H Influenzae' AND dose.vaccineName = 'H Influenzae' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F25" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VIP' AND d.vaccine = 'Pólio VIP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Pólio VIP' AND dose.vaccineName = 'Pólio VIP' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F26" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Pólio VOP' AND d.vaccine = 'Pólio VOP' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Pólio VOP' AND dose.vaccineName = 'Pólio VOP' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Rotavírus' AND d.vaccine = 'Rotavírus' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Rotavírus' AND dose.vaccineName = 'Rotavírus' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'VPC10' AND d.vaccine = 'VPC10' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'VPC10' AND dose.vaccineName = 'VPC10' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'ACWY/C' AND d.vaccine = 'ACWY/C' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'ACWY/C' AND dose.vaccineName = 'ACWY/C' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Meningocócica B' AND d.vaccine = 'Meningocócica B' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Meningocócica B' AND dose.vaccineName = 'Meningocócica B' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F31" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = '3V' AND d.vaccine = '3V' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = '3V' AND dose.vaccineName = '3V' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F32" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Febre amarela' AND d.vaccine = 'Febre amarela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Febre amarela' AND dose.vaccineName = 'Febre amarela' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Hepatite A' AND d.vaccine = 'Hepatite A' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Hepatite A' AND dose.vaccineName = 'Hepatite A' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'BCG' AND d.vaccine = 'BCG' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'BCG' AND dose.vaccineName = 'BCG' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'Varicela' AND d.vaccine = 'Varicela' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'Varicela' AND dose.vaccineName = 'Varicela' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F36" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'HPV4' AND d.vaccine = 'HPV4' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'HPV4' AND dose.vaccineName = 'HPV4' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" t="str">
         <f t="shared" si="2"/>
-        <v>MATCH (v:Vaccine), (d:VaccineDose) WHERE v.name = 'DTPa' AND d.vaccine = 'DTPa' MERGE (d)-[:IS_DOSE_OF]-&gt;(v);</v>
+        <v>MATCH (vac:Vaccine), (dose:VaccineDose) WHERE vac.name = 'DTPa' AND dose.vaccineName = 'DTPa' MERGE (dose)-[:IS_DOSE_OF]-&gt;(vac);</v>
       </c>
     </row>
   </sheetData>
@@ -3991,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391AE3A0-7DB7-4C1A-B882-6DBA4383A0D7}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G55"/>
+    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>